<commit_message>
Impl Einlesen Link State Updates
ausserdem: Code aufräumen, auskommentierten Code entfernen, Funktionen
dokumentieren
</commit_message>
<xml_diff>
--- a/doku/res/ospf_packages.xlsx
+++ b/doku/res/ospf_packages.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19700" tabRatio="797" activeTab="3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="93">
   <si>
     <t>Destination MAC</t>
   </si>
@@ -512,7 +512,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -733,8 +733,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="215">
+  <cellStyleXfs count="231">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -950,8 +959,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1286,8 +1311,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="215">
+  <cellStyles count="231">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -1395,6 +1432,14 @@
     <cellStyle name="Besuchter Link" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="230" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1502,6 +1547,14 @@
     <cellStyle name="Link" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="229" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
@@ -1535,15 +1588,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tabelle30" displayName="Tabelle30" ref="B2:G5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="30" name="Tabelle30" displayName="Tabelle30" ref="B2:G5" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="B2:G5"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Address" dataDxfId="7"/>
-    <tableColumn id="2" name="Interface" dataDxfId="6"/>
-    <tableColumn id="3" name="State" dataDxfId="5"/>
-    <tableColumn id="4" name="ID" dataDxfId="4"/>
-    <tableColumn id="5" name="Pri" dataDxfId="3"/>
-    <tableColumn id="6" name="Dead" dataDxfId="2"/>
+    <tableColumn id="1" name="Address" dataDxfId="5"/>
+    <tableColumn id="2" name="Interface" dataDxfId="4"/>
+    <tableColumn id="3" name="State" dataDxfId="3"/>
+    <tableColumn id="4" name="ID" dataDxfId="2"/>
+    <tableColumn id="5" name="Pri" dataDxfId="1"/>
+    <tableColumn id="6" name="Dead" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7192,10 +7245,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:AQ36"/>
+  <dimension ref="B2:AQ39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="AJ18" sqref="AJ18"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="AF39" sqref="AF39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.6640625" defaultRowHeight="28" customHeight="1" x14ac:dyDescent="0"/>
@@ -8660,7 +8713,88 @@
       <c r="AF36" s="3"/>
       <c r="AG36" s="3"/>
     </row>
+    <row r="37" spans="2:34" ht="28" customHeight="1">
+      <c r="B37" s="95"/>
+      <c r="C37" s="94"/>
+      <c r="E37" s="112" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="112"/>
+      <c r="G37" s="112"/>
+      <c r="H37" s="112"/>
+      <c r="I37" s="115"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="4"/>
+      <c r="M37" s="113" t="s">
+        <v>28</v>
+      </c>
+      <c r="N37" s="113"/>
+      <c r="O37" s="113"/>
+      <c r="P37" s="113"/>
+      <c r="Q37" s="114"/>
+      <c r="R37" s="26"/>
+      <c r="S37" s="11"/>
+      <c r="U37" s="112" t="s">
+        <v>29</v>
+      </c>
+      <c r="V37" s="112"/>
+      <c r="W37" s="112"/>
+      <c r="X37" s="112"/>
+      <c r="Y37" s="115"/>
+      <c r="Z37" s="29"/>
+      <c r="AA37" s="14"/>
+      <c r="AC37" s="112" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD37" s="112"/>
+      <c r="AE37" s="112"/>
+      <c r="AF37" s="112"/>
+      <c r="AG37" s="112"/>
+    </row>
+    <row r="39" spans="2:34" ht="28" customHeight="1">
+      <c r="B39" s="35"/>
+      <c r="C39" s="34"/>
+      <c r="E39" s="112" t="s">
+        <v>51</v>
+      </c>
+      <c r="F39" s="112"/>
+      <c r="G39" s="112"/>
+      <c r="H39" s="112"/>
+      <c r="I39" s="115"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="41"/>
+      <c r="M39" s="113" t="s">
+        <v>72</v>
+      </c>
+      <c r="N39" s="113"/>
+      <c r="O39" s="113"/>
+      <c r="P39" s="113"/>
+      <c r="Q39" s="113"/>
+      <c r="R39" s="66"/>
+      <c r="S39" s="65"/>
+      <c r="U39" s="113" t="s">
+        <v>73</v>
+      </c>
+      <c r="V39" s="113"/>
+      <c r="W39" s="113"/>
+      <c r="X39" s="113"/>
+      <c r="Y39" s="113"/>
+      <c r="Z39" s="56"/>
+      <c r="AA39" s="55"/>
+      <c r="AC39" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="AC37:AG37"/>
+    <mergeCell ref="E39:I39"/>
+    <mergeCell ref="M39:Q39"/>
+    <mergeCell ref="U39:Y39"/>
+    <mergeCell ref="M37:Q37"/>
+    <mergeCell ref="E37:I37"/>
+    <mergeCell ref="U37:Y37"/>
+  </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="45" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>